<commit_message>
feat: optimization slp & matrix games
</commit_message>
<xml_diff>
--- a/Оптимизация и принятие решений/Матричные игры/решение.xlsx
+++ b/Оптимизация и принятие решений/Матричные игры/решение.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tony_\OneDrive\Документы\omstu-works-2\Оптимизация и принятие решений\Матричные игры\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\omstu-works-2\Оптимизация и принятие решений\Матричные игры\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9273CBCF-8583-43CB-BF02-3227189EA5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20B4207-9C1E-48D0-9816-C090DE3AFEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
@@ -596,15 +596,15 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,7 +615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -637,7 +637,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>-2</v>
       </c>
@@ -655,7 +655,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -673,7 +673,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -694,7 +694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -703,7 +703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -712,7 +712,7 @@
         <v>НЕТ</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -742,7 +742,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -760,19 +760,19 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I11" s="1">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="J11" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -803,11 +803,11 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1">
         <f>SUMPRODUCT(H11:J11,H12:J12)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -836,13 +836,13 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1">
         <f>SUMPRODUCT(H11:J11,H13:J13)</f>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="M13" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G14" s="1"/>
       <c r="H14" s="1">
         <v>1</v>
@@ -856,13 +856,13 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1">
         <f>SUMPRODUCT(H11:J11,H14:J14)</f>
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="M14" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -897,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -914,7 +914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -944,7 +944,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G18" s="1"/>
       <c r="H18" s="1">
         <v>6</v>
@@ -959,7 +959,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -991,7 +991,7 @@
       </c>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G22" s="1"/>
       <c r="H22" s="1">
         <v>0</v>
@@ -1075,7 +1075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>14</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="6">
         <v>0.1111111111111111</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>5.5555555555555559E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="6">
         <f>B36*D39</f>
         <v>0.66666666666666663</v>
@@ -1212,7 +1212,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>16</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>17</v>
       </c>
@@ -1254,12 +1254,12 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>-2</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>НЕТ</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>14</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="6">
         <v>0</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="e">
         <f>B32*D35</f>
         <v>#DIV/0!</v>
@@ -1663,7 +1663,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>16</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>17</v>
       </c>

</xml_diff>